<commit_message>
Update AppChantier(add interface Sante Securite), journal de bord Nelson Cuervo
</commit_message>
<xml_diff>
--- a/NelsonCuervo/Sprint1/journal de bord Nelson Cuervo.xlsx
+++ b/NelsonCuervo/Sprint1/journal de bord Nelson Cuervo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\NelsonCuervo\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19354BB5-3B25-4213-813A-CBDD402175C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BBE140-F9E7-4CED-B386-1CFA46F519A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28770" yWindow="1680" windowWidth="28830" windowHeight="14655" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
+    <workbookView xWindow="0" yWindow="1545" windowWidth="28830" windowHeight="14655" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
-  <si>
-    <t>journal d'abord</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Nelson Alfonso Cuervo Caviedes</t>
   </si>
@@ -123,6 +120,15 @@
   </si>
   <si>
     <t>1h.</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">création de l'interface de la liste de contrôle santé sécurité </t>
+  </si>
+  <si>
+    <t>journal de bord</t>
   </si>
 </sst>
 </file>
@@ -138,15 +144,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,21 +166,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,15 +518,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72050F50-CF0C-4E9B-ADE3-1D6CB7D01C36}">
-  <dimension ref="B4:E26"/>
+  <dimension ref="B4:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="91.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -500,217 +534,251 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>44889</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>44890</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>44893</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>44894</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>44896</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>44898</v>
       </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>24</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>7</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <v>44900</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
+      <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>8</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <v>44902</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>27</v>
+      <c r="D25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>9</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <v>44903</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E26" t="s">
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>